<commit_message>
change diagram and pin-design
</commit_message>
<xml_diff>
--- a/Ele-diagram/引脚分配.xlsx
+++ b/Ele-diagram/引脚分配.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27904"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudsyehdudn\Desktop\机电系统设计实践\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47181505-9F76-4B7E-8AD4-D224C7A6E3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{27EFE26A-79A9-4549-B642-EF4A2A70FC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{848A23A3-E742-4412-AF67-59300162314B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -137,37 +139,52 @@
     <t>TIM1_CH2</t>
   </si>
   <si>
+    <t>OPENMV</t>
+  </si>
+  <si>
+    <t>OPENMV SG90</t>
+  </si>
+  <si>
+    <t>PE13</t>
+  </si>
+  <si>
+    <t>TIM1_CH3</t>
+  </si>
+  <si>
+    <t>脉冲测速</t>
+  </si>
+  <si>
+    <t>左轮电机编码器</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>TIM2_CH1</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>TIM2_CH2</t>
+  </si>
+  <si>
+    <t>右轮电机编码器</t>
+  </si>
+  <si>
+    <t>PD12</t>
+  </si>
+  <si>
     <t>TIM4_CH1</t>
   </si>
   <si>
-    <t>脉冲测速</t>
-  </si>
-  <si>
-    <t>左轮电机编码器</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>PA0</t>
-  </si>
-  <si>
-    <t>TIM2_CH1</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>PA1</t>
-  </si>
-  <si>
-    <t>TIM2_CH2</t>
-  </si>
-  <si>
-    <t>右轮电机编码器</t>
-  </si>
-  <si>
-    <t>PA6</t>
+    <t>PD13</t>
   </si>
   <si>
     <t>TIM4_CH2</t>
@@ -209,6 +226,9 @@
     <t>Echo</t>
   </si>
   <si>
+    <t>PA5</t>
+  </si>
+  <si>
     <t>TIM8_CH1</t>
   </si>
   <si>
@@ -281,9 +301,6 @@
     <t>串行通讯</t>
   </si>
   <si>
-    <t>OPENMV</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
@@ -302,6 +319,9 @@
     <t>USART1_RX</t>
   </si>
   <si>
+    <t>HC-06</t>
+  </si>
+  <si>
     <t>PC12</t>
   </si>
   <si>
@@ -327,31 +347,13 @@
   </si>
   <si>
     <t>USART3_RX</t>
-  </si>
-  <si>
-    <t>OPENMV SG90</t>
-  </si>
-  <si>
-    <t>TIM3_CH1</t>
-  </si>
-  <si>
-    <t>PD12</t>
-  </si>
-  <si>
-    <t>PD13</t>
-  </si>
-  <si>
-    <t>PA5</t>
-  </si>
-  <si>
-    <t>HC-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,10 +497,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -507,13 +512,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,7 +536,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -833,16 +835,16 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="17.59765625" customWidth="1"/>
-    <col min="5" max="5" width="13.59765625" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="14.25" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,11 +861,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="14.25" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -876,9 +878,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
+    <row r="3" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
@@ -889,9 +891,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9"/>
+    <row r="4" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
@@ -902,8 +904,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A5" s="8"/>
       <c r="B5" s="10"/>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -915,11 +917,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -932,8 +934,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A7" s="11"/>
       <c r="B7" s="10"/>
       <c r="C7" s="3" t="s">
         <v>20</v>
@@ -945,8 +947,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="9"/>
+    <row r="8" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -960,7 +962,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="26.25" thickBot="1">
       <c r="A9" s="10"/>
       <c r="B9" s="4" t="s">
         <v>27</v>
@@ -975,255 +977,262 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
-        <v>57</v>
+    <row r="10" spans="1:5" ht="14.25">
+      <c r="A10" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="5"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A13" s="7"/>
+      <c r="B13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1" thickBot="1">
       <c r="A15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="5"/>
-      <c r="B17" s="8" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="25.9" customHeight="1" thickBot="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="5"/>
-      <c r="B19" s="8" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="25.9" customHeight="1" thickBot="1">
+      <c r="A19" s="7"/>
+      <c r="B19" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A20" s="8"/>
       <c r="B20" s="10"/>
       <c r="C20" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="26.65" thickBot="1">
       <c r="A21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="5"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="26.65" thickBot="1">
+      <c r="A22" s="7"/>
       <c r="B22" s="10"/>
       <c r="C22" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="26.65" thickBot="1">
+      <c r="A23" s="7"/>
+      <c r="B23" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="5"/>
-      <c r="B23" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="5"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="26.65" thickBot="1">
+      <c r="A24" s="7"/>
       <c r="B24" s="10"/>
       <c r="C24" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="5"/>
-      <c r="B25" s="8" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="26.65" thickBot="1">
+      <c r="A25" s="7"/>
+      <c r="B25" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="7"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="26.65" thickBot="1">
+      <c r="A26" s="8"/>
       <c r="B26" s="10"/>
       <c r="C26" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
@@ -1232,13 +1241,6 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>